<commit_message>
last fixes for education menu and clickablilty of unvisible elements
</commit_message>
<xml_diff>
--- a/Icons/IconOverview.xlsx
+++ b/Icons/IconOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joellehelgert/Documents/FH/interactiveMedia/1Semester/termproject/Icons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17F0149-3113-EB4E-8A1A-789547258051}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB0BF92-CEA5-B74C-8317-AFD412415265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{85C7F068-B042-0145-8C35-C06A6D01B916}"/>
+    <workbookView xWindow="9000" yWindow="2120" windowWidth="35600" windowHeight="23900" xr2:uid="{85C7F068-B042-0145-8C35-C06A6D01B916}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t xml:space="preserve">Icon found </t>
   </si>
@@ -98,12 +98,27 @@
   <si>
     <t>youth center</t>
   </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Freetime</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Public Transport</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,12 +134,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -162,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -194,23 +224,346 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -246,7 +599,47 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -285,15 +678,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19686</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>385400</xdr:rowOff>
+          <xdr:rowOff>279400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -303,7 +696,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B68C322-AE6B-6340-809A-B9FA81D4A609}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -348,7 +741,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -360,7 +753,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -377,14 +770,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -393,7 +791,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2341E35B-543E-C144-9D56-CCFADE96C085}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -438,7 +836,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -450,7 +848,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -461,20 +859,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -483,7 +886,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2A5B61A-75DF-F749-8955-3C50A06FB158}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -528,7 +931,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -540,7 +943,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -551,20 +954,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
@@ -573,7 +981,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89183399-2C66-2140-B111-6744E719A1AD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -618,7 +1026,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -630,7 +1038,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -641,20 +1049,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
@@ -663,7 +1076,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D641BAE4-A251-804C-9265-6E11A356FDF9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -708,7 +1121,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -720,7 +1133,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -731,20 +1144,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
@@ -753,7 +1171,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E925BA5-EFB5-EA47-B284-5E76C7B9C9F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -798,7 +1216,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -810,7 +1228,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -821,20 +1239,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
@@ -843,7 +1266,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCFFAEF-832D-D44D-8C6C-6961770F03EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -888,7 +1311,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -900,7 +1323,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -911,20 +1334,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
@@ -933,7 +1361,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A35E8082-1961-9741-8A41-916EADB8A5FD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -978,7 +1406,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -990,7 +1418,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1001,20 +1429,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
@@ -1023,7 +1456,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D94DDFAF-7E4E-8B40-8CF0-FB6F4F6A64D7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1068,7 +1501,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1080,7 +1513,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1091,20 +1524,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
@@ -1113,7 +1551,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD7DE8FF-47F5-6E45-8CE5-7E2A839E95FA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1158,7 +1596,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1170,7 +1608,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1181,20 +1619,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="19686" cy="360000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
@@ -1203,7 +1646,7 @@
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40CBC379-DACD-DA4A-9EF3-6DB018D39212}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1248,7 +1691,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1260,7 +1703,7 @@
               <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
-              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1271,7 +1714,7 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1293,7 +1736,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7DD1B54-33A0-FE4E-934E-80F290420A0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1337,7 +1780,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73E96ECC-81B2-F14C-A7FB-03990CD8D2AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1381,7 +1824,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{180E3BD9-BDA1-9D49-B60A-2C46C444B18F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1425,7 +1868,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBD7E40F-A2A6-9F4D-9B93-A60F10187D2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1469,7 +1912,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AAEA61-3B99-6F4E-9F6D-A002BA4468CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1513,7 +1956,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D902163-F373-4B47-A7BD-B6C114861DC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1557,7 +2000,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B42B139-5990-2441-BA3F-1DF8748ADCDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1601,7 +2044,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3378D45B-2A59-A042-9A7B-50A11B190D1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1645,7 +2088,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E249EF1-E52F-5541-AAE5-C2D613303C3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1689,7 +2132,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66ED9752-9BD0-7D45-B061-D24ADD1B16CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1733,7 +2176,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{126CF111-0641-B34C-84EA-D138C0CAC5C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1759,6 +2202,1296 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1065" name="Check Box 41" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1065"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E70B8829-1954-974A-B306-203FD5DF9D8D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>418144</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133691</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C44E13-C458-4E41-910C-AD33365A7840}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8242983" y="2154766"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1066" name="Check Box 42" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1066"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{877CBA47-2397-B14C-A683-A228EDC25CA3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>353689</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71420</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB635AD9-4BD6-444B-BC73-E23DFBC36CE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15539065" y="2092495"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1067" name="Check Box 43" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1067"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD74D8F-B687-F340-9A64-20C63E9B81A9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>312721</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68553</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="357269"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B55A2A74-2406-4344-B872-A469A7493F99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13586269" y="2089628"/>
+          <a:ext cx="360000" cy="357269"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1069" name="Check Box 45" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1069"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3644479E-D046-DC4F-99CC-5936E6A976B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EDEC66C-8B7D-7546-A09B-4DDA61AF385A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="355600" y="6164826"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1070" name="Check Box 46" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1070"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD3AF31-3FC5-DF4C-9943-93CE0E1AD8B3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6E39516-BE4F-FB4F-A85D-5A4BB7E25921}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="6682795"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1071" name="Check Box 47" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1071"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7278C58C-D227-EA45-B0BE-1036F3E3671A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>392290</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>87489</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="374111"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{690D2C96-2078-444B-89D1-0B1E3DF4D162}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="392290" y="7666521"/>
+          <a:ext cx="360000" cy="374111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1072" name="Check Box 48" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1072"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A022C2-17A7-8A46-A426-FD45EF542EF5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>346996</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>77156</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61F1A15A-D379-FE4D-927F-7DE80960B404}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13620544" y="3614038"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1074" name="Check Box 50" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1074"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D37B5B4-6E31-0F4D-8512-D9E94C0C5563}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6E49005-09C2-6948-A8E0-1BD20AAA0DB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="4598219"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1075" name="Check Box 51" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1075"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2BB987E-1301-0A4C-AA03-8C4CE0DA9740}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>370212</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>106379</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFD4CC7A-6810-DD45-99F8-5AD3F99012A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8195051" y="5159067"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>25400</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="25400" cy="254000"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1077" name="Check Box 53" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1077"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79F24E3D-B2F4-3340-B7BE-E22201510919}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>369256</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80023</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="360000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297125DA-FE4B-3B4F-8B33-3162953C899B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13642804" y="5132711"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2059,180 +3792,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18F641A-1195-A741-9629-51EB8F02039B}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.1640625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="43.5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="35.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="34.5" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="40" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:14" ht="40" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:14" ht="40" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="32"/>
     </row>
-    <row r="4" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:14" ht="40" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="33"/>
     </row>
-    <row r="5" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="40" customHeight="1">
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="19"/>
     </row>
-    <row r="6" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="40" customHeight="1">
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:14" ht="40" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="15"/>
+      <c r="M7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+    <row r="8" spans="1:14" ht="40" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:14" ht="40" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="34"/>
     </row>
-    <row r="10" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="40" customHeight="1">
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="34"/>
     </row>
-    <row r="11" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="40" customHeight="1">
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="34"/>
     </row>
-    <row r="12" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="40" customHeight="1">
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="36"/>
     </row>
-    <row r="13" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="40" customHeight="1">
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="35"/>
     </row>
-    <row r="14" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="40" customHeight="1">
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+    <row r="15" spans="1:14" ht="40" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:14" ht="40" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+    <row r="17" spans="1:4" ht="40" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+    <row r="18" spans="1:4" ht="40" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+    <row r="19" spans="1:4" ht="40" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+    <row r="20" spans="1:4" ht="40" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" customHeight="1">
       <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="J7:J9"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A7:A9"/>
@@ -2307,7 +4204,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>279400</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2490,6 +4387,226 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1065" r:id="rId14" name="Check Box 41">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1066" r:id="rId15" name="Check Box 42">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1067" r:id="rId16" name="Check Box 43">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1069" r:id="rId17" name="Check Box 45">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1070" r:id="rId18" name="Check Box 46">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1071" r:id="rId19" name="Check Box 47">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1072" r:id="rId20" name="Check Box 48">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1074" r:id="rId21" name="Check Box 50">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1075" r:id="rId22" name="Check Box 51">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1077" r:id="rId23" name="Check Box 53">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>25400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>279400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>